<commit_message>
fix: import excel, generate QR codes, and render PDF
</commit_message>
<xml_diff>
--- a/public/file.xlsx
+++ b/public/file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\admin-desa\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66A6ABC8-E7E7-4330-9AD7-4672631EC294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760BC716-8628-499A-88C6-FA983C4BF372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{10A5B482-F740-4FB0-8491-E0CDCC5F9C88}"/>
+    <workbookView xWindow="10620" yWindow="0" windowWidth="9870" windowHeight="10920" xr2:uid="{10A5B482-F740-4FB0-8491-E0CDCC5F9C88}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>harmanto</t>
+  </si>
+  <si>
+    <t>Khumaidah</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,172 +413,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52776963-5895-40AA-8D82-AC725A2494EC}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1">
+        <v>141341</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>3030000</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-      <c r="E1">
-        <v>1</v>
-      </c>
-      <c r="F1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>6</v>
-      </c>
-      <c r="E6">
-        <v>6</v>
-      </c>
-      <c r="F6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>7</v>
-      </c>
-      <c r="D7">
-        <v>7</v>
-      </c>
-      <c r="E7">
-        <v>7</v>
-      </c>
-      <c r="F7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>8</v>
-      </c>
-      <c r="E8">
-        <v>8</v>
-      </c>
-      <c r="F8">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>